<commit_message>
modified new data raw file
</commit_message>
<xml_diff>
--- a/Data/Raw Data/berliner-toiletten-SANIFAIR_Rail.xlsx
+++ b/Data/Raw Data/berliner-toiletten-SANIFAIR_Rail.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\agnan\techlabs\st-22 pedom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joma\Techlabs\st22-peedom\Data\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CA83B7-8D60-4BBA-BE5E-D3BB39711036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8E50CE-6F63-4929-8364-9AE571003621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,7 +304,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.000000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -389,7 +389,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B22" sqref="B21:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,10 +816,10 @@
         <v>18</v>
       </c>
       <c r="H5" s="8">
-        <v>13.388736093261301</v>
+        <v>13.388736093</v>
       </c>
       <c r="I5" s="8">
-        <v>52.548913457549801</v>
+        <v>52.548913458000001</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -833,8 +833,14 @@
       <c r="M5">
         <v>1</v>
       </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
       <c r="P5">
         <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>6</v>
       </c>
       <c r="R5">
         <v>1</v>
@@ -860,10 +866,10 @@
         <v>18</v>
       </c>
       <c r="H6" s="8">
-        <v>13.3885166696226</v>
+        <v>13.38851667</v>
       </c>
       <c r="I6" s="8">
-        <v>52.549209000176901</v>
+        <v>52.549208999999998</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -877,14 +883,20 @@
       <c r="M6">
         <v>1</v>
       </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
       <c r="P6">
         <v>1</v>
       </c>
+      <c r="Q6">
+        <v>6</v>
+      </c>
       <c r="R6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -904,10 +916,10 @@
         <v>18</v>
       </c>
       <c r="H7" s="8">
-        <v>13.334153322834201</v>
+        <v>13.334153323000001</v>
       </c>
       <c r="I7" s="8">
-        <v>52.508296523435597</v>
+        <v>52.508296522999999</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -921,14 +933,20 @@
       <c r="M7">
         <v>1</v>
       </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
       <c r="P7">
         <v>0</v>
       </c>
+      <c r="Q7">
+        <v>6</v>
+      </c>
       <c r="R7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -948,10 +966,10 @@
         <v>18</v>
       </c>
       <c r="H8" s="8">
-        <v>13.3872499236899</v>
+        <v>13.387249924000001</v>
       </c>
       <c r="I8" s="8">
-        <v>52.519966530132599</v>
+        <v>52.519966529999998</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -965,14 +983,20 @@
       <c r="M8">
         <v>1</v>
       </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
       <c r="P8">
         <v>1</v>
       </c>
+      <c r="Q8">
+        <v>6</v>
+      </c>
       <c r="R8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -992,10 +1016,10 @@
         <v>18</v>
       </c>
       <c r="H9" s="8">
-        <v>13.411754707332999</v>
+        <v>13.411754707</v>
       </c>
       <c r="I9" s="8">
-        <v>52.5213985760277</v>
+        <v>52.521398576000003</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1009,14 +1033,20 @@
       <c r="M9">
         <v>1</v>
       </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
       <c r="P9">
         <v>1</v>
       </c>
+      <c r="Q9">
+        <v>6</v>
+      </c>
       <c r="R9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1036,10 +1066,10 @@
         <v>18</v>
       </c>
       <c r="H10" s="8">
-        <v>13.1910261793331</v>
+        <v>13.191026179</v>
       </c>
       <c r="I10" s="8">
-        <v>52.434341540571701</v>
+        <v>52.434341541000002</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1053,14 +1083,20 @@
       <c r="M10">
         <v>1</v>
       </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
       <c r="P10">
         <v>1</v>
       </c>
+      <c r="Q10">
+        <v>6</v>
+      </c>
       <c r="R10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -1080,10 +1116,10 @@
         <v>18</v>
       </c>
       <c r="H11" s="8">
-        <v>13.467933001007401</v>
+        <v>13.467933001</v>
       </c>
       <c r="I11" s="8">
-        <v>52.503972643799301</v>
+        <v>52.503972644000001</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1097,14 +1133,20 @@
       <c r="M11">
         <v>1</v>
       </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
       <c r="P11">
         <v>1</v>
       </c>
+      <c r="Q11">
+        <v>6</v>
+      </c>
       <c r="R11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -1124,10 +1166,10 @@
         <v>18</v>
       </c>
       <c r="H12" s="8">
-        <v>13.497256016243201</v>
+        <v>13.497256016</v>
       </c>
       <c r="I12" s="8">
-        <v>52.509409104236902</v>
+        <v>52.509409104</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1138,8 +1180,23 @@
       <c r="L12" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>6</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -1159,10 +1216,10 @@
         <v>18</v>
       </c>
       <c r="H13" s="8">
-        <v>13.1792963294966</v>
+        <v>13.179296329</v>
       </c>
       <c r="I13" s="8">
-        <v>52.4215857146038</v>
+        <v>52.421585714999999</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1176,8 +1233,14 @@
       <c r="M13">
         <v>1</v>
       </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
       <c r="P13">
         <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>6</v>
       </c>
       <c r="R13">
         <v>1</v>
@@ -1203,10 +1266,10 @@
         <v>18</v>
       </c>
       <c r="H14" s="8">
-        <v>13.199195978747101</v>
+        <v>13.199195979000001</v>
       </c>
       <c r="I14" s="8">
-        <v>52.534650505857499</v>
+        <v>52.534650505999998</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1220,8 +1283,14 @@
       <c r="M14">
         <v>1</v>
       </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
       <c r="P14">
         <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>6</v>
       </c>
       <c r="R14">
         <v>1</v>
@@ -1247,10 +1316,10 @@
         <v>18</v>
       </c>
       <c r="H15" s="8">
-        <v>13.365804842405201</v>
+        <v>13.365804841999999</v>
       </c>
       <c r="I15" s="8">
-        <v>52.476169622327198</v>
+        <v>52.476169622</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1264,8 +1333,14 @@
       <c r="M15">
         <v>1</v>
       </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
       <c r="P15">
         <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>6</v>
       </c>
       <c r="R15">
         <v>1</v>
@@ -1291,10 +1366,10 @@
         <v>18</v>
       </c>
       <c r="H16" s="8">
-        <v>13.3641734956857</v>
+        <v>13.364173495999999</v>
       </c>
       <c r="I16" s="8">
-        <v>52.476434922963101</v>
+        <v>52.476434922999999</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1308,8 +1383,14 @@
       <c r="M16">
         <v>1</v>
       </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
       <c r="P16">
         <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>6</v>
       </c>
       <c r="R16">
         <v>1</v>
@@ -1335,10 +1416,10 @@
         <v>18</v>
       </c>
       <c r="H17" s="8">
-        <v>13.435104375188301</v>
+        <v>13.435104375</v>
       </c>
       <c r="I17" s="8">
-        <v>52.510225528319701</v>
+        <v>52.510225527999999</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1352,14 +1433,20 @@
       <c r="M17">
         <v>1</v>
       </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
       <c r="P17">
         <v>1</v>
       </c>
+      <c r="Q17">
+        <v>6</v>
+      </c>
       <c r="R17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1379,10 +1466,10 @@
         <v>18</v>
       </c>
       <c r="H18" s="8">
-        <v>13.3759468130368</v>
+        <v>13.375946813000001</v>
       </c>
       <c r="I18" s="8">
-        <v>52.509646781043003</v>
+        <v>52.509646781000001</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -1396,8 +1483,14 @@
       <c r="M18">
         <v>1</v>
       </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
       <c r="P18">
         <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>6</v>
       </c>
       <c r="R18">
         <v>1</v>
@@ -1423,10 +1516,10 @@
         <v>18</v>
       </c>
       <c r="H19" s="8">
-        <v>13.368468334086501</v>
+        <v>13.368468333999999</v>
       </c>
       <c r="I19" s="8">
-        <v>52.525689797341499</v>
+        <v>52.525689796999998</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -1440,8 +1533,17 @@
       <c r="M19">
         <v>1</v>
       </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
       <c r="P19">
         <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>6</v>
       </c>
       <c r="R19">
         <v>1</v>

</xml_diff>